<commit_message>
XTag API of New
</commit_message>
<xml_diff>
--- a/zero-ambient/src/main/resources/plugin/ambient/oob/cab/x.tag.xlsx
+++ b/zero-ambient/src/main/resources/plugin/ambient/oob/cab/x.tag.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lang/Develop/Source/ox-workshop/vertx-zero/vertx-pin/zero-ambient/src/main/resources/plugin/ambient/oob/cab/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lang/zero-cloud/web-app/workshop/zero-ws/zero-extension/zero-ambient/src/main/resources/plugin/ambient/oob/cab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF12B82F-73E8-EA40-9A9E-5641303A8C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7378F23E-DE00-FC4D-B369-691A50E6400D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="71540" yWindow="-4000" windowWidth="38400" windowHeight="22560" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
+    <workbookView xWindow="-46700" yWindow="-13880" windowWidth="38400" windowHeight="22560" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA-PERM" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="190">
   <si>
     <t>key</t>
   </si>
@@ -607,37 +607,55 @@
   </si>
   <si>
     <t>302e001f-5e99-468e-8187-fdca3aee2f88</t>
+  </si>
+  <si>
+    <t>res.tag.by.model</t>
+  </si>
+  <si>
+    <t>读取模型标签</t>
+  </si>
+  <si>
+    <t>a0ea8356-18e2-4529-be66-b65131f8b156</t>
+  </si>
+  <si>
+    <t>fb34ed83-eccc-4cb0-8af4-75ae786fa67a</t>
+  </si>
+  <si>
+    <t>act.tag.by.model</t>
+  </si>
+  <si>
+    <t>/api/x-tag/m/:identifier/:key</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
       <color rgb="FF0070C0"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -645,14 +663,14 @@
     <font>
       <sz val="16"/>
       <color rgb="FF0070C0"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -778,7 +796,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -786,7 +804,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1187,1393 +1204,1439 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D6C9C3-8DFE-A442-A082-10767386D931}">
-  <dimension ref="A2:K64"/>
+  <dimension ref="A2:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:A62"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="21"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="54.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="51.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11" style="4"/>
-    <col min="14" max="14" width="63.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="11" style="4"/>
+    <col min="1" max="1" width="54.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="54.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="51.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" style="3"/>
+    <col min="14" max="14" width="63.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="11" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="5" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="7" t="s">
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="10" t="s">
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="10" t="s">
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="10" t="s">
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="10" t="s">
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="10" t="s">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="10" t="s">
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="5" t="s">
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="7" t="s">
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="10" t="s">
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="10" t="s">
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="10" t="s">
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="10" t="s">
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="10" t="s">
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="10" t="s">
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="23" t="s">
+      <c r="C25" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="5" t="s">
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="G26" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="H26" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I26" s="5" t="s">
+      <c r="I26" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="7" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="17" t="s">
+      <c r="D27" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F27" s="17" t="s">
+      <c r="F27" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G27" s="7" t="s">
+      <c r="G27" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H27" s="7" t="s">
+      <c r="H27" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I27" s="7" t="s">
+      <c r="I27" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="10" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="B28" s="16" t="str">
-        <f t="shared" ref="B28:B42" si="0">A48</f>
+      <c r="B28" s="15" t="str">
+        <f t="shared" ref="B28:B43" si="0">A49</f>
         <v>0258b6a9-50b2-4092-bd3c-bc944c6c2713</v>
       </c>
-      <c r="C28" s="16" t="str">
+      <c r="C28" s="15" t="str">
         <f>A15</f>
         <v>644384d6-d9d5-4c97-9341-be9f25043874</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="E28" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F28" s="13" t="s">
+      <c r="F28" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="G28" s="12" t="s">
+      <c r="G28" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="H28" s="12">
+      <c r="H28" s="11">
         <v>1</v>
       </c>
-      <c r="I28" s="12"/>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="10" t="s">
+      <c r="I28" s="11"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="B29" s="16" t="str">
+      <c r="B29" s="15" t="str">
         <f t="shared" si="0"/>
         <v>d679b170-118a-4b1c-8e78-500f490b2cba</v>
       </c>
-      <c r="C29" s="16" t="str">
+      <c r="C29" s="15" t="str">
         <f>A16</f>
         <v>7ab047be-760c-4af3-8466-a29570a445a5</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="E29" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F29" s="13" t="s">
+      <c r="F29" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="G29" s="12" t="s">
+      <c r="G29" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="H29" s="12">
+      <c r="H29" s="11">
         <v>4</v>
       </c>
-      <c r="I29" s="12"/>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="10" t="s">
+      <c r="I29" s="11"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="B30" s="16" t="str">
+      <c r="B30" s="15" t="str">
         <f t="shared" si="0"/>
         <v>bbcb1b08-d09a-4987-997d-c3876b26c6e8</v>
       </c>
-      <c r="C30" s="16" t="str">
+      <c r="C30" s="15" t="str">
         <f>A17</f>
         <v>0ddbfc8b-3e06-4d9a-9a79-be01b877e582</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="E30" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F30" s="13" t="s">
+      <c r="F30" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="G30" s="12" t="s">
+      <c r="G30" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="H30" s="12">
+      <c r="H30" s="11">
         <v>8</v>
       </c>
-      <c r="I30" s="12"/>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="10" t="s">
+      <c r="I30" s="11"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="B31" s="16" t="str">
+      <c r="B31" s="15" t="str">
         <f t="shared" si="0"/>
         <v>cb52dce7-20dc-4d90-8790-5a423cec8a0f</v>
       </c>
-      <c r="C31" s="16" t="str">
+      <c r="C31" s="15" t="str">
         <f>A18</f>
         <v>5dd11ab0-d079-44b6-94e3-c53262080f2e</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="E31" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F31" s="13" t="s">
+      <c r="F31" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="G31" s="12" t="s">
+      <c r="G31" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="H31" s="12">
+      <c r="H31" s="11">
         <v>12</v>
       </c>
-      <c r="I31" s="12"/>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="10" t="s">
+      <c r="I31" s="11"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="B32" s="16" t="str">
+      <c r="B32" s="15" t="str">
         <f t="shared" si="0"/>
         <v>8e25d5a6-8438-4ba2-a0de-0ecc0c0a1c2d</v>
       </c>
-      <c r="C32" s="16" t="str">
+      <c r="C32" s="15" t="str">
         <f>A15</f>
         <v>644384d6-d9d5-4c97-9341-be9f25043874</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D32" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="E32" s="12" t="s">
+      <c r="E32" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F32" s="13" t="s">
+      <c r="F32" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="G32" s="12" t="s">
+      <c r="G32" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="H32" s="12">
+      <c r="H32" s="11">
         <v>1</v>
       </c>
-      <c r="I32" s="12"/>
-    </row>
-    <row r="33" spans="1:11">
-      <c r="A33" s="10" t="s">
+      <c r="I32" s="11"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="B33" s="16" t="str">
+      <c r="B33" s="15" t="str">
         <f t="shared" si="0"/>
         <v>1897ed48-aa85-48ac-bc9c-1f45078c4206</v>
       </c>
-      <c r="C33" s="16" t="str">
+      <c r="C33" s="15" t="str">
         <f>A17</f>
         <v>0ddbfc8b-3e06-4d9a-9a79-be01b877e582</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="D33" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="E33" s="12" t="s">
+      <c r="E33" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F33" s="13" t="s">
+      <c r="F33" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="G33" s="12" t="s">
+      <c r="G33" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="H33" s="12">
+      <c r="H33" s="11">
         <v>8</v>
       </c>
-      <c r="I33" s="12"/>
-    </row>
-    <row r="34" spans="1:11">
-      <c r="A34" s="10" t="s">
+      <c r="I33" s="11"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="B34" s="16" t="str">
+      <c r="B34" s="15" t="str">
         <f t="shared" si="0"/>
         <v>acfd08e7-cec2-4431-884e-ae1a5f15e549</v>
       </c>
-      <c r="C34" s="16" t="str">
+      <c r="C34" s="15" t="str">
         <f>A18</f>
         <v>5dd11ab0-d079-44b6-94e3-c53262080f2e</v>
       </c>
-      <c r="D34" s="13" t="s">
+      <c r="D34" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="E34" s="12" t="s">
+      <c r="E34" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F34" s="13" t="s">
+      <c r="F34" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="G34" s="12" t="s">
+      <c r="G34" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="H34" s="12">
+      <c r="H34" s="11">
         <v>12</v>
       </c>
-      <c r="I34" s="12"/>
-    </row>
-    <row r="35" spans="1:11">
-      <c r="A35" s="10" t="s">
+      <c r="I34" s="11"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="B35" s="16" t="str">
+      <c r="B35" s="15" t="str">
         <f t="shared" si="0"/>
         <v>c0845a02-56e7-4d6b-9e8a-49f1646579ed</v>
       </c>
-      <c r="C35" s="16" t="str">
+      <c r="C35" s="15" t="str">
         <f>A19</f>
         <v>c48f2d56-2f0f-4906-8330-eb799d2d1a47</v>
       </c>
-      <c r="D35" s="13" t="s">
+      <c r="D35" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="E35" s="12" t="s">
+      <c r="E35" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F35" s="13" t="s">
+      <c r="F35" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="G35" s="12" t="s">
+      <c r="G35" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="H35" s="12">
+      <c r="H35" s="11">
         <v>3</v>
       </c>
-      <c r="I35" s="12"/>
-    </row>
-    <row r="36" spans="1:11">
-      <c r="A36" s="10" t="s">
+      <c r="I35" s="11"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="B36" s="16" t="str">
+      <c r="B36" s="15" t="str">
         <f t="shared" si="0"/>
         <v>9ef3ceda-e2a3-4adf-b94c-97523da4c0af</v>
       </c>
-      <c r="C36" s="16" t="str">
+      <c r="C36" s="15" t="str">
         <f>A19</f>
         <v>c48f2d56-2f0f-4906-8330-eb799d2d1a47</v>
       </c>
-      <c r="D36" s="13" t="s">
+      <c r="D36" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="E36" s="12" t="s">
+      <c r="E36" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F36" s="13" t="s">
+      <c r="F36" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="G36" s="12" t="s">
+      <c r="G36" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="H36" s="12">
+      <c r="H36" s="11">
         <v>3</v>
       </c>
-      <c r="I36" s="12"/>
-    </row>
-    <row r="37" spans="1:11">
-      <c r="A37" s="10" t="s">
+      <c r="I36" s="11"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="B37" s="16" t="str">
+      <c r="B37" s="15" t="str">
         <f t="shared" si="0"/>
         <v>a3511c8a-0be9-40a8-83dd-53fa95efa6f6</v>
       </c>
-      <c r="C37" s="16" t="str">
+      <c r="C37" s="15" t="str">
         <f>A19</f>
         <v>c48f2d56-2f0f-4906-8330-eb799d2d1a47</v>
       </c>
-      <c r="D37" s="13" t="s">
+      <c r="D37" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="E37" s="12" t="s">
+      <c r="E37" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F37" s="13" t="s">
+      <c r="F37" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="G37" s="12" t="s">
+      <c r="G37" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="H37" s="12">
+      <c r="H37" s="11">
         <v>11</v>
       </c>
-      <c r="I37" s="12"/>
-    </row>
-    <row r="38" spans="1:11">
-      <c r="A38" s="10" t="s">
+      <c r="I37" s="11"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="B38" s="16" t="str">
+      <c r="B38" s="15" t="str">
         <f t="shared" si="0"/>
         <v>aabbb7c0-dfb4-4260-a8a0-13365dfb6e56</v>
       </c>
-      <c r="C38" s="16" t="str">
+      <c r="C38" s="15" t="str">
         <f>A20</f>
         <v>2e359266-f41e-4d55-aac6-1651c90126bf</v>
       </c>
-      <c r="D38" s="13" t="s">
+      <c r="D38" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="E38" s="12" t="s">
+      <c r="E38" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F38" s="13" t="s">
+      <c r="F38" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="G38" s="12" t="s">
+      <c r="G38" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="H38" s="12">
+      <c r="H38" s="11">
         <v>5</v>
       </c>
-      <c r="I38" s="12"/>
-    </row>
-    <row r="39" spans="1:11">
-      <c r="A39" s="10" t="s">
+      <c r="I38" s="11"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="B39" s="16" t="str">
+      <c r="B39" s="15" t="str">
         <f t="shared" si="0"/>
         <v>68946e6b-e429-4386-bccd-f744aefc922a</v>
       </c>
-      <c r="C39" s="16" t="str">
+      <c r="C39" s="15" t="str">
         <f>A20</f>
         <v>2e359266-f41e-4d55-aac6-1651c90126bf</v>
       </c>
-      <c r="D39" s="13" t="s">
+      <c r="D39" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="E39" s="12" t="s">
+      <c r="E39" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F39" s="13" t="s">
+      <c r="F39" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="G39" s="12" t="s">
+      <c r="G39" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="H39" s="12">
+      <c r="H39" s="11">
         <v>3</v>
       </c>
-      <c r="I39" s="12"/>
-    </row>
-    <row r="40" spans="1:11">
-      <c r="A40" s="10" t="s">
+      <c r="I39" s="11"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="B40" s="16" t="str">
+      <c r="B40" s="15" t="str">
         <f t="shared" si="0"/>
         <v>61b767c4-573a-414c-addd-f2917d0edd24</v>
       </c>
-      <c r="C40" s="16" t="str">
+      <c r="C40" s="15" t="str">
         <f>A15</f>
         <v>644384d6-d9d5-4c97-9341-be9f25043874</v>
       </c>
-      <c r="D40" s="13" t="s">
+      <c r="D40" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="E40" s="12" t="s">
+      <c r="E40" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F40" s="13" t="s">
+      <c r="F40" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="G40" s="12" t="s">
+      <c r="G40" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="H40" s="12">
+      <c r="H40" s="11">
         <v>1</v>
       </c>
-      <c r="I40" s="12"/>
-    </row>
-    <row r="41" spans="1:11">
-      <c r="A41" s="10" t="s">
+      <c r="I40" s="11"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="B41" s="16" t="str">
+      <c r="B41" s="15" t="str">
         <f t="shared" si="0"/>
         <v>72d89820-5775-4045-bd0e-0311b1dae572</v>
       </c>
-      <c r="C41" s="16" t="str">
+      <c r="C41" s="15" t="str">
         <f>A15</f>
         <v>644384d6-d9d5-4c97-9341-be9f25043874</v>
       </c>
-      <c r="D41" s="13" t="s">
+      <c r="D41" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="E41" s="12" t="s">
+      <c r="E41" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F41" s="13" t="s">
+      <c r="F41" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="G41" s="12" t="s">
+      <c r="G41" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="H41" s="12">
+      <c r="H41" s="11">
         <v>1</v>
       </c>
-      <c r="I41" s="12"/>
-    </row>
-    <row r="42" spans="1:11">
-      <c r="A42" s="10" t="s">
+      <c r="I41" s="11"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="B42" s="16" t="str">
+      <c r="B42" s="15" t="str">
         <f t="shared" si="0"/>
         <v>302e001f-5e99-468e-8187-fdca3aee2f88</v>
       </c>
-      <c r="C42" s="16" t="str">
-        <f>A15</f>
+      <c r="C42" s="15" t="str">
+        <f>A$15</f>
         <v>644384d6-d9d5-4c97-9341-be9f25043874</v>
       </c>
-      <c r="D42" s="13" t="s">
+      <c r="D42" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="E42" s="12" t="s">
+      <c r="E42" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F42" s="13" t="s">
+      <c r="F42" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="G42" s="12" t="s">
+      <c r="G42" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="H42" s="12">
+      <c r="H42" s="11">
         <v>2</v>
       </c>
-      <c r="I42" s="12"/>
-    </row>
-    <row r="43" spans="1:11">
-      <c r="A43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="15"/>
-      <c r="G43" s="4"/>
-      <c r="K43" s="14"/>
-    </row>
-    <row r="44" spans="1:11">
-      <c r="A44" s="14"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="15"/>
-      <c r="G44" s="4"/>
-      <c r="K44" s="14"/>
-    </row>
-    <row r="45" spans="1:11">
-      <c r="A45" s="1" t="s">
+      <c r="I42" s="11"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="B43" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>a0ea8356-18e2-4529-be66-b65131f8b156</v>
+      </c>
+      <c r="C43" s="15" t="str">
+        <f>A$15</f>
+        <v>644384d6-d9d5-4c97-9341-be9f25043874</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F43" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="H43" s="11">
+        <v>2</v>
+      </c>
+      <c r="I43" s="11"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="13"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="3"/>
+      <c r="K44" s="13"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="3"/>
+      <c r="K45" s="13"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C45" s="21" t="s">
+      <c r="C46" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D45" s="22"/>
-      <c r="E45" s="22"/>
-      <c r="F45" s="22"/>
-      <c r="G45" s="22"/>
-      <c r="H45" s="22"/>
-      <c r="I45" s="22"/>
-      <c r="J45" s="22"/>
-      <c r="K45" s="22"/>
-    </row>
-    <row r="46" spans="1:11">
-      <c r="A46" s="5" t="s">
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
+      <c r="K46" s="21"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B47" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C46" s="18" t="s">
+      <c r="C47" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D47" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="E47" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F46" s="6" t="s">
+      <c r="F47" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G46" s="18" t="s">
+      <c r="G47" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="H46" s="18" t="s">
+      <c r="H47" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="I46" s="18" t="s">
+      <c r="I47" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="J46" s="5" t="s">
+      <c r="J47" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="K46" s="5" t="s">
+      <c r="K47" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
-      <c r="A47" s="7" t="s">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B48" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C48" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D47" s="17" t="s">
+      <c r="D48" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E47" s="9" t="s">
+      <c r="E48" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F47" s="9" t="s">
+      <c r="F48" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="G47" s="7" t="s">
+      <c r="G48" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H47" s="7" t="s">
+      <c r="H48" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="I47" s="7" t="s">
+      <c r="I48" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="J47" s="7" t="s">
+      <c r="J48" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="K47" s="7" t="s">
+      <c r="K48" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
-      <c r="A48" s="10" t="s">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="B48" s="12" t="s">
+      <c r="B49" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="C48" s="12" t="s">
+      <c r="C49" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D48" s="13" t="s">
+      <c r="D49" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="E48" s="12" t="s">
+      <c r="E49" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F48" s="12" t="s">
+      <c r="F49" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G48" s="12">
+      <c r="G49" s="11">
         <v>1</v>
       </c>
-      <c r="H48" s="12"/>
-      <c r="I48" s="12"/>
-      <c r="J48" s="11" t="b">
+      <c r="H49" s="11"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="K48" s="11" t="s">
+      <c r="K49" s="10" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
-      <c r="A49" s="10" t="s">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="B49" s="12" t="s">
+      <c r="B50" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="C49" s="12" t="s">
+      <c r="C50" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D49" s="13" t="s">
+      <c r="D50" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="E49" s="12" t="s">
+      <c r="E50" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F49" s="12" t="s">
+      <c r="F50" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G49" s="12">
+      <c r="G50" s="11">
         <v>4</v>
       </c>
-      <c r="H49" s="12"/>
-      <c r="I49" s="12"/>
-      <c r="J49" s="11"/>
-      <c r="K49" s="11"/>
-    </row>
-    <row r="50" spans="1:11">
-      <c r="A50" s="10" t="s">
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="10"/>
+      <c r="K50" s="10"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="B50" s="12" t="s">
+      <c r="B51" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="C50" s="12" t="s">
+      <c r="C51" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D50" s="13" t="s">
+      <c r="D51" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="E50" s="12" t="s">
+      <c r="E51" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F50" s="12" t="s">
+      <c r="F51" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G50" s="12">
+      <c r="G51" s="11">
         <v>8</v>
       </c>
-      <c r="H50" s="12"/>
-      <c r="I50" s="12"/>
-      <c r="J50" s="11"/>
-      <c r="K50" s="11"/>
-    </row>
-    <row r="51" spans="1:11">
-      <c r="A51" s="10" t="s">
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="10"/>
+      <c r="K51" s="10"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="B51" s="12" t="s">
+      <c r="B52" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="C51" s="12" t="s">
+      <c r="C52" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D51" s="13" t="s">
+      <c r="D52" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="E51" s="12" t="s">
+      <c r="E52" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F51" s="12" t="s">
+      <c r="F52" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G51" s="12">
+      <c r="G52" s="11">
         <v>12</v>
       </c>
-      <c r="H51" s="12"/>
-      <c r="I51" s="12"/>
-      <c r="J51" s="11"/>
-      <c r="K51" s="11"/>
-    </row>
-    <row r="52" spans="1:11">
-      <c r="A52" s="10" t="s">
+      <c r="H52" s="11"/>
+      <c r="I52" s="11"/>
+      <c r="J52" s="10"/>
+      <c r="K52" s="10"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="B52" s="12" t="s">
+      <c r="B53" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="C52" s="12" t="s">
+      <c r="C53" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D52" s="13" t="s">
+      <c r="D53" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="E52" s="12" t="s">
+      <c r="E53" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F52" s="12" t="s">
+      <c r="F53" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G52" s="12">
+      <c r="G53" s="11">
         <v>1</v>
       </c>
-      <c r="H52" s="12"/>
-      <c r="I52" s="12"/>
-      <c r="J52" s="11"/>
-      <c r="K52" s="11"/>
-    </row>
-    <row r="53" spans="1:11">
-      <c r="A53" s="10" t="s">
+      <c r="H53" s="11"/>
+      <c r="I53" s="11"/>
+      <c r="J53" s="10"/>
+      <c r="K53" s="10"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="B53" s="12" t="s">
+      <c r="B54" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="C53" s="12" t="s">
+      <c r="C54" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D53" s="13" t="s">
+      <c r="D54" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E53" s="12" t="s">
+      <c r="E54" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F53" s="12" t="s">
+      <c r="F54" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G53" s="12">
+      <c r="G54" s="11">
         <v>8</v>
       </c>
-      <c r="H53" s="12"/>
-      <c r="I53" s="12"/>
-      <c r="J53" s="11"/>
-      <c r="K53" s="11"/>
-    </row>
-    <row r="54" spans="1:11">
-      <c r="A54" s="10" t="s">
+      <c r="H54" s="11"/>
+      <c r="I54" s="11"/>
+      <c r="J54" s="10"/>
+      <c r="K54" s="10"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="B54" s="12" t="s">
+      <c r="B55" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="C54" s="12" t="s">
+      <c r="C55" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D54" s="13" t="s">
+      <c r="D55" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="E54" s="12" t="s">
+      <c r="E55" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F54" s="12" t="s">
+      <c r="F55" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G54" s="12">
+      <c r="G55" s="11">
         <v>12</v>
       </c>
-      <c r="H54" s="12"/>
-      <c r="I54" s="12"/>
-      <c r="J54" s="11"/>
-      <c r="K54" s="11"/>
-    </row>
-    <row r="55" spans="1:11">
-      <c r="A55" s="10" t="s">
+      <c r="H55" s="11"/>
+      <c r="I55" s="11"/>
+      <c r="J55" s="10"/>
+      <c r="K55" s="10"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="B55" s="12" t="s">
+      <c r="B56" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="C55" s="12" t="s">
+      <c r="C56" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D55" s="13" t="s">
+      <c r="D56" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="E55" s="12" t="s">
+      <c r="E56" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F55" s="12" t="s">
+      <c r="F56" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G55" s="12">
+      <c r="G56" s="11">
         <v>3</v>
       </c>
-      <c r="H55" s="12"/>
-      <c r="I55" s="12"/>
-      <c r="J55" s="11"/>
-      <c r="K55" s="11"/>
-    </row>
-    <row r="56" spans="1:11">
-      <c r="A56" s="10" t="s">
+      <c r="H56" s="11"/>
+      <c r="I56" s="11"/>
+      <c r="J56" s="10"/>
+      <c r="K56" s="10"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="B56" s="12" t="s">
+      <c r="B57" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="C56" s="12" t="s">
+      <c r="C57" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D56" s="13" t="s">
+      <c r="D57" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="E56" s="12" t="s">
+      <c r="E57" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F56" s="12" t="s">
+      <c r="F57" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G56" s="12">
+      <c r="G57" s="11">
         <v>3</v>
       </c>
-      <c r="H56" s="12"/>
-      <c r="I56" s="12"/>
-      <c r="J56" s="11"/>
-      <c r="K56" s="11"/>
-    </row>
-    <row r="57" spans="1:11">
-      <c r="A57" s="10" t="s">
+      <c r="H57" s="11"/>
+      <c r="I57" s="11"/>
+      <c r="J57" s="10"/>
+      <c r="K57" s="10"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="B57" s="12" t="s">
+      <c r="B58" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="C57" s="12" t="s">
+      <c r="C58" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D57" s="13" t="s">
+      <c r="D58" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="E57" s="12" t="s">
+      <c r="E58" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F57" s="12" t="s">
+      <c r="F58" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G57" s="12">
+      <c r="G58" s="11">
         <v>11</v>
       </c>
-      <c r="H57" s="12"/>
-      <c r="I57" s="12"/>
-      <c r="J57" s="11"/>
-      <c r="K57" s="11"/>
-    </row>
-    <row r="58" spans="1:11">
-      <c r="A58" s="10" t="s">
+      <c r="H58" s="11"/>
+      <c r="I58" s="11"/>
+      <c r="J58" s="10"/>
+      <c r="K58" s="10"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="B58" s="12" t="s">
+      <c r="B59" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="C58" s="12" t="s">
+      <c r="C59" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D58" s="13" t="s">
+      <c r="D59" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="E58" s="12" t="s">
+      <c r="E59" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F58" s="12" t="s">
+      <c r="F59" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G58" s="12">
+      <c r="G59" s="11">
         <v>5</v>
       </c>
-      <c r="H58" s="12"/>
-      <c r="I58" s="12"/>
-      <c r="J58" s="11"/>
-      <c r="K58" s="11"/>
-    </row>
-    <row r="59" spans="1:11">
-      <c r="A59" s="10" t="s">
+      <c r="H59" s="11"/>
+      <c r="I59" s="11"/>
+      <c r="J59" s="10"/>
+      <c r="K59" s="10"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="B59" s="12" t="s">
+      <c r="B60" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="C59" s="12" t="s">
+      <c r="C60" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D59" s="13" t="s">
+      <c r="D60" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="E59" s="12" t="s">
+      <c r="E60" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F59" s="12" t="s">
+      <c r="F60" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G59" s="12">
+      <c r="G60" s="11">
         <v>3</v>
       </c>
-      <c r="H59" s="12"/>
-      <c r="I59" s="12"/>
-      <c r="J59" s="11"/>
-      <c r="K59" s="11"/>
-    </row>
-    <row r="60" spans="1:11">
-      <c r="A60" s="10" t="s">
+      <c r="H60" s="11"/>
+      <c r="I60" s="11"/>
+      <c r="J60" s="10"/>
+      <c r="K60" s="10"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="B60" s="12" t="s">
+      <c r="B61" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="C60" s="12" t="s">
+      <c r="C61" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D60" s="13" t="s">
+      <c r="D61" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="E60" s="12" t="s">
+      <c r="E61" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F60" s="12" t="s">
+      <c r="F61" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G60" s="12">
+      <c r="G61" s="11">
         <v>1</v>
       </c>
-      <c r="H60" s="12"/>
-      <c r="I60" s="12"/>
-      <c r="J60" s="11"/>
-      <c r="K60" s="11"/>
-    </row>
-    <row r="61" spans="1:11">
-      <c r="A61" s="10" t="s">
+      <c r="H61" s="11"/>
+      <c r="I61" s="11"/>
+      <c r="J61" s="10"/>
+      <c r="K61" s="10"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="B61" s="12" t="s">
+      <c r="B62" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="C61" s="12" t="s">
+      <c r="C62" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D61" s="13" t="s">
+      <c r="D62" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="E61" s="12" t="s">
+      <c r="E62" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F61" s="12" t="s">
+      <c r="F62" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G61" s="12">
+      <c r="G62" s="11">
         <v>1</v>
       </c>
-      <c r="H61" s="12"/>
-      <c r="I61" s="12"/>
-      <c r="J61" s="11"/>
-      <c r="K61" s="11"/>
-    </row>
-    <row r="62" spans="1:11">
-      <c r="A62" s="10" t="s">
+      <c r="H62" s="11"/>
+      <c r="I62" s="11"/>
+      <c r="J62" s="10"/>
+      <c r="K62" s="10"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="B62" s="12" t="s">
+      <c r="B63" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="C62" s="12" t="s">
+      <c r="C63" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D62" s="13" t="s">
+      <c r="D63" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="E62" s="12" t="s">
+      <c r="E63" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F62" s="12" t="s">
+      <c r="F63" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G62" s="12">
+      <c r="G63" s="11">
         <v>2</v>
       </c>
-      <c r="H62" s="12"/>
-      <c r="I62" s="12"/>
-      <c r="J62" s="11"/>
-      <c r="K62" s="11"/>
-    </row>
-    <row r="63" spans="1:11">
-      <c r="A63" s="14"/>
-      <c r="C63" s="14"/>
-      <c r="D63" s="15"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="15"/>
-      <c r="G63" s="4"/>
-      <c r="K63" s="14"/>
-    </row>
-    <row r="64" spans="1:11">
-      <c r="A64" s="14"/>
-      <c r="D64" s="4"/>
-      <c r="E64" s="4"/>
-      <c r="G64" s="4"/>
-      <c r="K64" s="14"/>
+      <c r="H63" s="11"/>
+      <c r="I63" s="11"/>
+      <c r="J63" s="10"/>
+      <c r="K63" s="10"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="C64" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="E64" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F64" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G64" s="11">
+        <v>2</v>
+      </c>
+      <c r="H64" s="11"/>
+      <c r="I64" s="11"/>
+      <c r="J64" s="10"/>
+      <c r="K64" s="10"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" s="13"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="G65" s="3"/>
+      <c r="K65" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C45:K45"/>
+    <mergeCell ref="C46:K46"/>
     <mergeCell ref="C25:I25"/>
     <mergeCell ref="C2:D2"/>
   </mergeCells>

</xml_diff>